<commit_message>
added occupation + attributes fixtures with import-manager
</commit_message>
<xml_diff>
--- a/static/fixtures/all_fixtures.xlsx
+++ b/static/fixtures/all_fixtures.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\hackathon-career-track\backend\static\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474E2C3B-9584-40F4-8E55-85E5D2EB8DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD509DA-320A-4F27-9665-5BE2729E92AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8C1FF65F-BB85-46BD-84F6-9B812959FAAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{8C1FF65F-BB85-46BD-84F6-9B812959FAAA}"/>
   </bookViews>
   <sheets>
     <sheet name="direction" sheetId="6" r:id="rId1"/>
     <sheet name="course" sheetId="1" r:id="rId2"/>
     <sheet name="city" sheetId="2" r:id="rId3"/>
     <sheet name="stack" sheetId="4" r:id="rId4"/>
-    <sheet name="work_status" sheetId="5" r:id="rId5"/>
-    <sheet name="course-stack" sheetId="3" r:id="rId6"/>
+    <sheet name="activity" sheetId="5" r:id="rId5"/>
+    <sheet name="format" sheetId="7" r:id="rId6"/>
+    <sheet name="occupation" sheetId="8" r:id="rId7"/>
+    <sheet name="review_status" sheetId="9" r:id="rId8"/>
+    <sheet name="course-stack" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="425">
   <si>
     <t>Дизайнер интерфейсов</t>
   </si>
@@ -1281,6 +1284,39 @@
   </si>
   <si>
     <t>direction_id</t>
+  </si>
+  <si>
+    <t>удаленка</t>
+  </si>
+  <si>
+    <t>офис</t>
+  </si>
+  <si>
+    <t>гибрид</t>
+  </si>
+  <si>
+    <t>полная</t>
+  </si>
+  <si>
+    <t>неполный день</t>
+  </si>
+  <si>
+    <t>стажировка</t>
+  </si>
+  <si>
+    <t>Не выбрано</t>
+  </si>
+  <si>
+    <t>На рассмотрении</t>
+  </si>
+  <si>
+    <t>Отправлено тестовое</t>
+  </si>
+  <si>
+    <t>Отказ</t>
+  </si>
+  <si>
+    <t>Назначено собеседование</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A8C534-EF10-409C-909B-AB8A76229C2C}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -5103,6 +5139,166 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684CCCEF-EC2B-491A-8EE6-F21562A34FB7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0DEBF9-DE60-471B-8F11-89C5873F7DAF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC8FA61-4F88-47AB-BC79-36955EBB3665}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F63FA5-8127-4E71-AEF4-423371477418}">
   <dimension ref="A1:B282"/>
   <sheetViews>

</xml_diff>